<commit_message>
update data to remove student names
</commit_message>
<xml_diff>
--- a/aspartic.xlsx
+++ b/aspartic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ewueagles-my.sharepoint.com/personal/rmcrae_ewu_edu/Documents/titrator/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C3D91A-6673-4B2C-9F7B-9DE4E209DEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{91C3D91A-6673-4B2C-9F7B-9DE4E209DEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B78EC15-136A-4F2C-A54C-A531C247F0B1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1305" yWindow="30" windowWidth="25590" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
-    <t>Jayslin Shrader and Natalie Potter</t>
-  </si>
-  <si>
     <t>Unknown # 1</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>pH</t>
+  </si>
+  <si>
+    <t>names here</t>
   </si>
 </sst>
 </file>
@@ -2923,9 +2923,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2963,7 +2963,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3069,7 +3069,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3211,7 +3211,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3225,47 +3225,47 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>